<commit_message>
Connection settings more error checking
</commit_message>
<xml_diff>
--- a/doc/Serial_Packets.xlsx
+++ b/doc/Serial_Packets.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WORK\Projects\Astrohn\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -65,9 +60,6 @@
     <t>Запросить версию SW</t>
   </si>
   <si>
-    <t>Сирийный номер</t>
-  </si>
-  <si>
     <t>LEN_0 = 0xХХ</t>
   </si>
   <si>
@@ -75,12 +67,15 @@
   </si>
   <si>
     <t>Data_n</t>
+  </si>
+  <si>
+    <t>Серийный номер</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -211,7 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -481,7 +476,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -492,7 +487,7 @@
   <dimension ref="B2:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +557,7 @@
         <v>7</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -618,7 +613,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>4</v>
@@ -627,10 +622,10 @@
         <v>5</v>
       </c>
       <c r="H11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new types of packets add NIOS(SW) registers
</commit_message>
<xml_diff>
--- a/doc/Serial_Packets.xlsx
+++ b/doc/Serial_Packets.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7815"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Packet Format" sheetId="1" r:id="rId1"/>
+    <sheet name="SW_ADDR" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="93">
   <si>
     <t>SYNC_1 = 0x5A</t>
   </si>
@@ -117,13 +118,199 @@
   </si>
   <si>
     <t>Модуль занят и не может обработать пакет</t>
+  </si>
+  <si>
+    <t>Prm_ADDR_0</t>
+  </si>
+  <si>
+    <t>Prm_ADDR_1</t>
+  </si>
+  <si>
+    <t>PKG_TYPE = 0x3</t>
+  </si>
+  <si>
+    <t>RD\WRn</t>
+  </si>
+  <si>
+    <t>DATA_0</t>
+  </si>
+  <si>
+    <t>DATA_1</t>
+  </si>
+  <si>
+    <t>DATA_2</t>
+  </si>
+  <si>
+    <t>DATA_3</t>
+  </si>
+  <si>
+    <t>0x0 - WR</t>
+  </si>
+  <si>
+    <t>0x1 - RD</t>
+  </si>
+  <si>
+    <t>поля только для записи</t>
+  </si>
+  <si>
+    <t>LEN_0 = 0xC</t>
+  </si>
+  <si>
+    <t>RD_LEN = 0x8</t>
+  </si>
+  <si>
+    <t>Запись/чтение  параметра в SW области</t>
+  </si>
+  <si>
+    <t>Response RD</t>
+  </si>
+  <si>
+    <t>Request WR</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>0x0000</t>
+  </si>
+  <si>
+    <t>EPCS Flash Start address</t>
+  </si>
+  <si>
+    <t>0x0001</t>
+  </si>
+  <si>
+    <t>Total Lenth(bytes) of WR/RD operations</t>
+  </si>
+  <si>
+    <t>0x0002</t>
+  </si>
+  <si>
+    <t>EPCS ID</t>
+  </si>
+  <si>
+    <t>0x0003</t>
+  </si>
+  <si>
+    <t>0x0004</t>
+  </si>
+  <si>
+    <t>0x0005</t>
+  </si>
+  <si>
+    <t>0x0006</t>
+  </si>
+  <si>
+    <t>0x0007</t>
+  </si>
+  <si>
+    <t>0x0008</t>
+  </si>
+  <si>
+    <t>0x0009</t>
+  </si>
+  <si>
+    <t>0x0010</t>
+  </si>
+  <si>
+    <t>0x0011</t>
+  </si>
+  <si>
+    <t>0x0012</t>
+  </si>
+  <si>
+    <t>0x0013</t>
+  </si>
+  <si>
+    <t>0x0014</t>
+  </si>
+  <si>
+    <t>0x0015</t>
+  </si>
+  <si>
+    <t>0x0016</t>
+  </si>
+  <si>
+    <t>0x0017</t>
+  </si>
+  <si>
+    <t>0x0018</t>
+  </si>
+  <si>
+    <t>0x0019</t>
+  </si>
+  <si>
+    <t>0x0020</t>
+  </si>
+  <si>
+    <t>0x0021</t>
+  </si>
+  <si>
+    <t>0x0022</t>
+  </si>
+  <si>
+    <t>0x0023</t>
+  </si>
+  <si>
+    <t>0x0024</t>
+  </si>
+  <si>
+    <t>R/W</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Пакетная запись в буфер</t>
+  </si>
+  <si>
+    <t>PKG_TYPE = 0x4</t>
+  </si>
+  <si>
+    <t>1024+5</t>
+  </si>
+  <si>
+    <t>DATA_1024</t>
+  </si>
+  <si>
+    <t>DATA…</t>
+  </si>
+  <si>
+    <t>……</t>
+  </si>
+  <si>
+    <t>LEN_0 = 0x00</t>
+  </si>
+  <si>
+    <t>LEN_1 = 0x4</t>
+  </si>
+  <si>
+    <t>0x400 - 1024 байта</t>
+  </si>
+  <si>
+    <t>EPCS command 0x0 - null; 0x1 - WR; 0x2 - RD ; 0x3 - erase sector</t>
+  </si>
+  <si>
+    <t>0x5</t>
+  </si>
+  <si>
+    <t>Неправильная команда</t>
+  </si>
+  <si>
+    <t>0x6</t>
+  </si>
+  <si>
+    <t>Неизвестный тип пакета</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,8 +351,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,11 +419,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -281,6 +500,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -288,7 +544,7 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -319,15 +575,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -611,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection sqref="A1:L42"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,25 +913,25 @@
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="38.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="10" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -779,16 +1070,16 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
@@ -922,17 +1213,33 @@
         <v>30</v>
       </c>
     </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F30" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G30" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F31" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="G31" t="s">
+        <v>92</v>
+      </c>
+    </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
     </row>
     <row r="40" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
@@ -978,20 +1285,476 @@
       <c r="E42" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F42" s="10" t="s">
+      <c r="F42" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G42" s="10" t="s">
+      <c r="G42" s="17" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <v>1</v>
+      </c>
+      <c r="B50" s="7">
+        <v>2</v>
+      </c>
+      <c r="C50" s="7">
+        <v>3</v>
+      </c>
+      <c r="D50" s="7">
+        <v>4</v>
+      </c>
+      <c r="E50" s="7">
+        <v>5</v>
+      </c>
+      <c r="F50" s="7">
+        <v>6</v>
+      </c>
+      <c r="G50" s="7">
+        <v>7</v>
+      </c>
+      <c r="H50" s="7">
+        <v>8</v>
+      </c>
+      <c r="I50" s="7">
+        <v>9</v>
+      </c>
+      <c r="J50" s="7">
+        <v>10</v>
+      </c>
+      <c r="K50" s="7">
+        <v>11</v>
+      </c>
+      <c r="L50" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I51" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J51" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K51" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L51" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D52" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I52" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="J52" s="21"/>
+      <c r="K52" s="21"/>
+      <c r="L52" s="22"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F53" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B56" s="18"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+    </row>
+    <row r="57" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
+        <v>1</v>
+      </c>
+      <c r="B58" s="7">
+        <v>2</v>
+      </c>
+      <c r="C58" s="7">
+        <v>3</v>
+      </c>
+      <c r="D58" s="7">
+        <v>4</v>
+      </c>
+      <c r="E58" s="7">
+        <v>5</v>
+      </c>
+      <c r="F58" s="7">
+        <v>6</v>
+      </c>
+      <c r="G58" s="7">
+        <v>7</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I58" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G59" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I59" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D60" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F60" s="13"/>
+      <c r="I60" s="29"/>
+      <c r="J60" s="29"/>
+      <c r="K60" s="29"/>
+      <c r="L60" s="29"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F61" s="13"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
+    <mergeCell ref="A56:H56"/>
+    <mergeCell ref="I60:L60"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A39:H39"/>
     <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A48:H48"/>
+    <mergeCell ref="I52:L52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="65.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="28"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="28"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="25"/>
+      <c r="C8" s="28"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="28"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="25"/>
+      <c r="C10" s="28"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="28"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="28"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="28"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="25"/>
+      <c r="C14" s="28"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="25"/>
+      <c r="C15" s="28"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="25"/>
+      <c r="C16" s="28"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="25"/>
+      <c r="C17" s="28"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="25"/>
+      <c r="C18" s="28"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="25"/>
+      <c r="C19" s="28"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="25"/>
+      <c r="C20" s="28"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="25"/>
+      <c r="C21" s="28"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="25"/>
+      <c r="C22" s="28"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="25"/>
+      <c r="C23" s="28"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="25"/>
+      <c r="C24" s="28"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="25"/>
+      <c r="C25" s="28"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="25"/>
+      <c r="C26" s="28"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
--added cmd=0x4 update firmware --added epcs_prog instruction
</commit_message>
<xml_diff>
--- a/doc/Serial_Packets.xlsx
+++ b/doc/Serial_Packets.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WORK\Projects\Astrohn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WORK\Projects\Astrohn\Astrohn_S_DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7815"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Packet Format" sheetId="1" r:id="rId1"/>
@@ -291,9 +291,6 @@
     <t>0x400 - 1024 байта</t>
   </si>
   <si>
-    <t>EPCS command 0x0 - null; 0x1 - WR; 0x2 - RD ; 0x3 - erase sector</t>
-  </si>
-  <si>
     <t>0x5</t>
   </si>
   <si>
@@ -304,6 +301,9 @@
   </si>
   <si>
     <t>Неизвестный тип пакета</t>
+  </si>
+  <si>
+    <t>EPCS command 0x0 - null; 0x1 - WR; 0x2 - RD ; 0x3 - erase sector;  0x4-update FW</t>
   </si>
 </sst>
 </file>
@@ -585,9 +585,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -600,25 +619,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -904,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56:H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,16 +922,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -1070,16 +1070,16 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
@@ -1215,31 +1215,31 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F30" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G30" t="s">
         <v>89</v>
-      </c>
-      <c r="G30" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F31" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="G31" t="s">
         <v>91</v>
       </c>
-      <c r="G31" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
     </row>
     <row r="40" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
@@ -1293,16 +1293,16 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
@@ -1395,12 +1395,12 @@
       <c r="F52" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I52" s="20" t="s">
+      <c r="I52" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="J52" s="21"/>
-      <c r="K52" s="21"/>
-      <c r="L52" s="22"/>
+      <c r="J52" s="28"/>
+      <c r="K52" s="28"/>
+      <c r="L52" s="29"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F53" s="13" t="s">
@@ -1408,16 +1408,16 @@
       </c>
     </row>
     <row r="56" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="18" t="s">
+      <c r="A56" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="B56" s="18"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="24"/>
+      <c r="H56" s="24"/>
     </row>
     <row r="57" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
@@ -1490,10 +1490,10 @@
         <v>87</v>
       </c>
       <c r="F60" s="13"/>
-      <c r="I60" s="29"/>
-      <c r="J60" s="29"/>
-      <c r="K60" s="29"/>
-      <c r="L60" s="29"/>
+      <c r="I60" s="25"/>
+      <c r="J60" s="25"/>
+      <c r="K60" s="25"/>
+      <c r="L60" s="25"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F61" s="13"/>
@@ -1517,217 +1517,217 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.7109375" customWidth="1"/>
-    <col min="2" max="2" width="65.140625" customWidth="1"/>
+    <col min="2" max="2" width="107.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="22" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="23" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="23" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="23" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="28" t="s">
+      <c r="B5" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="28"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="28"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="23"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="28"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="23"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="28"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="23"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="28"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="23"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="28"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="23"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="28"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="23"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="28"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="23"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="28"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="23"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="28"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="23"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="28"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="23"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="28"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="23"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="28"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="23"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="28"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="23"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="28"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="23"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="28"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="23"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="28"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="23"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="28"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="23"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="28"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="23"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="28"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="23"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="28"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="23"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>

</xml_diff>

<commit_message>
added nios files upd serial protocol
</commit_message>
<xml_diff>
--- a/doc/Serial_Packets.xlsx
+++ b/doc/Serial_Packets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7815" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Packet Format" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="95">
   <si>
     <t>SYNC_1 = 0x5A</t>
   </si>
@@ -153,9 +153,6 @@
     <t>поля только для записи</t>
   </si>
   <si>
-    <t>LEN_0 = 0xC</t>
-  </si>
-  <si>
     <t>RD_LEN = 0x8</t>
   </si>
   <si>
@@ -304,6 +301,15 @@
   </si>
   <si>
     <t>EPCS command 0x0 - null; 0x1 - WR; 0x2 - RD ; 0x3 - erase sector;  0x4-update FW</t>
+  </si>
+  <si>
+    <t>LEN_0 = 0x7</t>
+  </si>
+  <si>
+    <t>0x7</t>
+  </si>
+  <si>
+    <t>Ошибка записи регистра SW</t>
   </si>
 </sst>
 </file>
@@ -904,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:H56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,18 +1221,26 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F30" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" t="s">
         <v>88</v>
-      </c>
-      <c r="G30" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F31" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G31" t="s">
         <v>90</v>
       </c>
-      <c r="G31" t="s">
-        <v>91</v>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F32" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1294,7 +1308,7 @@
     </row>
     <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B48" s="24"/>
       <c r="C48" s="24"/>
@@ -1306,10 +1320,10 @@
     </row>
     <row r="49" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -1361,7 +1375,7 @@
         <v>33</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>4</v>
@@ -1390,7 +1404,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D52" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F52" s="13" t="s">
         <v>39</v>
@@ -1409,7 +1423,7 @@
     </row>
     <row r="56" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B56" s="24"/>
       <c r="C56" s="24"/>
@@ -1421,10 +1435,10 @@
     </row>
     <row r="57" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
@@ -1450,10 +1464,10 @@
         <v>7</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I58" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
@@ -1464,13 +1478,13 @@
         <v>0</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D59" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="F59" s="15" t="s">
         <v>35</v>
@@ -1479,15 +1493,15 @@
         <v>36</v>
       </c>
       <c r="H59" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I59" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D60" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F60" s="13"/>
       <c r="I60" s="25"/>
@@ -1517,8 +1531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,202 +1543,202 @@
   <sheetData>
     <row r="1" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>48</v>
-      </c>
       <c r="C1" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="23"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="23"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="23"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="20"/>
       <c r="C10" s="23"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="23"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="23"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" s="23"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="23"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" s="20"/>
       <c r="C15" s="23"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="23"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B17" s="20"/>
       <c r="C17" s="23"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B18" s="20"/>
       <c r="C18" s="23"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="23"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20" s="20"/>
       <c r="C20" s="23"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B21" s="20"/>
       <c r="C21" s="23"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B22" s="20"/>
       <c r="C22" s="23"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B23" s="20"/>
       <c r="C23" s="23"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B24" s="20"/>
       <c r="C24" s="23"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B25" s="20"/>
       <c r="C25" s="23"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" s="20"/>
       <c r="C26" s="23"/>

</xml_diff>

<commit_message>
added Firmware Alpication start BOOT address register
</commit_message>
<xml_diff>
--- a/doc/Serial_Packets.xlsx
+++ b/doc/Serial_Packets.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="96">
   <si>
     <t>SYNC_1 = 0x5A</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>EPCS command 0x0 - null; 0x1 - WR; 0x2 - RD ; 0x3 - erase sector;  0x4-update FW ;  0x5-read FW</t>
+  </si>
+  <si>
+    <t>Firmware Alpication start BOOT address</t>
   </si>
 </sst>
 </file>
@@ -550,7 +553,7 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -624,6 +627,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1532,7 +1538,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1600,8 +1606,12 @@
       <c r="A6" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">

</xml_diff>

<commit_message>
added Remote Upgrades register
</commit_message>
<xml_diff>
--- a/doc/Serial_Packets.xlsx
+++ b/doc/Serial_Packets.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="138">
   <si>
     <t>SYNC_1 = 0x5A</t>
   </si>
@@ -313,6 +313,132 @@
   </si>
   <si>
     <t>Firmware Alpication start BOOT address</t>
+  </si>
+  <si>
+    <t>0x0025</t>
+  </si>
+  <si>
+    <t>0x0026</t>
+  </si>
+  <si>
+    <t>0x0027</t>
+  </si>
+  <si>
+    <t>0x0028</t>
+  </si>
+  <si>
+    <t>0x0029</t>
+  </si>
+  <si>
+    <t>0x0030</t>
+  </si>
+  <si>
+    <t>0x0031</t>
+  </si>
+  <si>
+    <t>0x0032</t>
+  </si>
+  <si>
+    <t>0x0033</t>
+  </si>
+  <si>
+    <t>0x0034</t>
+  </si>
+  <si>
+    <t>0x0035</t>
+  </si>
+  <si>
+    <t>0x0036</t>
+  </si>
+  <si>
+    <t>0x0037</t>
+  </si>
+  <si>
+    <t>0x0038</t>
+  </si>
+  <si>
+    <t>0x0039</t>
+  </si>
+  <si>
+    <t>0x0040</t>
+  </si>
+  <si>
+    <t>0x0041</t>
+  </si>
+  <si>
+    <t>0x0042</t>
+  </si>
+  <si>
+    <t>0x0043</t>
+  </si>
+  <si>
+    <t>0x0044</t>
+  </si>
+  <si>
+    <t>0x0045</t>
+  </si>
+  <si>
+    <t>0x0046</t>
+  </si>
+  <si>
+    <t>0x0047</t>
+  </si>
+  <si>
+    <t>0x0048</t>
+  </si>
+  <si>
+    <t>0x0049</t>
+  </si>
+  <si>
+    <t>0x0050</t>
+  </si>
+  <si>
+    <t>0x0051</t>
+  </si>
+  <si>
+    <t>0x0052</t>
+  </si>
+  <si>
+    <t>0x0053</t>
+  </si>
+  <si>
+    <t>0x0054</t>
+  </si>
+  <si>
+    <t>0x0055</t>
+  </si>
+  <si>
+    <t>0x0056</t>
+  </si>
+  <si>
+    <t>0x0057</t>
+  </si>
+  <si>
+    <t>0x0058</t>
+  </si>
+  <si>
+    <t>0x0059</t>
+  </si>
+  <si>
+    <t>0x0060</t>
+  </si>
+  <si>
+    <t>0x0061</t>
+  </si>
+  <si>
+    <t>0x0062</t>
+  </si>
+  <si>
+    <t>Set Boot Address: 0x0  - Factory;  Firmware Alpication start BOOT address(read from rg_addr= 0x4) - application</t>
+  </si>
+  <si>
+    <t>Remote System Upgrade</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>0x1 - Jump to Boot Address</t>
   </si>
 </sst>
 </file>
@@ -553,7 +679,7 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -612,6 +738,9 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -628,8 +757,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -934,16 +1063,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -1082,16 +1211,16 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
@@ -1250,16 +1379,16 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="24" t="s">
+      <c r="A39" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
     </row>
     <row r="40" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
@@ -1313,16 +1442,16 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="24" t="s">
+      <c r="A48" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="24"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="25"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
@@ -1415,12 +1544,12 @@
       <c r="F52" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I52" s="27" t="s">
+      <c r="I52" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="J52" s="28"/>
-      <c r="K52" s="28"/>
-      <c r="L52" s="29"/>
+      <c r="J52" s="29"/>
+      <c r="K52" s="29"/>
+      <c r="L52" s="30"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F53" s="13" t="s">
@@ -1428,16 +1557,16 @@
       </c>
     </row>
     <row r="56" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="24" t="s">
+      <c r="A56" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
-      <c r="D56" s="24"/>
-      <c r="E56" s="24"/>
-      <c r="F56" s="24"/>
-      <c r="G56" s="24"/>
-      <c r="H56" s="24"/>
+      <c r="B56" s="25"/>
+      <c r="C56" s="25"/>
+      <c r="D56" s="25"/>
+      <c r="E56" s="25"/>
+      <c r="F56" s="25"/>
+      <c r="G56" s="25"/>
+      <c r="H56" s="25"/>
     </row>
     <row r="57" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
@@ -1510,10 +1639,10 @@
         <v>86</v>
       </c>
       <c r="F60" s="13"/>
-      <c r="I60" s="25"/>
-      <c r="J60" s="25"/>
-      <c r="K60" s="25"/>
-      <c r="L60" s="25"/>
+      <c r="I60" s="26"/>
+      <c r="J60" s="26"/>
+      <c r="K60" s="26"/>
+      <c r="L60" s="26"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F61" s="13"/>
@@ -1535,10 +1664,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,7 +1735,7 @@
       <c r="A6" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="24" t="s">
         <v>95</v>
       </c>
       <c r="C6" s="23" t="s">
@@ -1691,91 +1820,346 @@
       <c r="C17" s="23"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="23"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="31"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="23"/>
+        <v>67</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="23"/>
+        <v>68</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" s="20"/>
       <c r="C21" s="23"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" s="20"/>
       <c r="C22" s="23"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" s="20"/>
       <c r="C23" s="23"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" s="20"/>
       <c r="C24" s="23"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="20"/>
       <c r="C25" s="23"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="20"/>
       <c r="C26" s="23"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
+      <c r="A27" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="20"/>
+      <c r="C27" s="23"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="23"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
+      <c r="A29" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="23"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
+      <c r="A30" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" s="20"/>
+      <c r="C30" s="23"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
+      <c r="A31" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" s="20"/>
+      <c r="C31" s="23"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
+      <c r="A32" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="20"/>
+      <c r="C32" s="23"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="20"/>
+      <c r="C33" s="23"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B34" s="20"/>
+      <c r="C34" s="23"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" s="20"/>
+      <c r="C35" s="23"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="20"/>
+      <c r="C36" s="23"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" s="20"/>
+      <c r="C37" s="23"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" s="20"/>
+      <c r="C38" s="23"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" s="20"/>
+      <c r="C39" s="23"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" s="20"/>
+      <c r="C40" s="23"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="20"/>
+      <c r="C41" s="23"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B42" s="20"/>
+      <c r="C42" s="23"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" s="20"/>
+      <c r="C43" s="23"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" s="20"/>
+      <c r="C44" s="23"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B45" s="20"/>
+      <c r="C45" s="23"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B46" s="20"/>
+      <c r="C46" s="23"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B47" s="20"/>
+      <c r="C47" s="23"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B48" s="20"/>
+      <c r="C48" s="23"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B49" s="20"/>
+      <c r="C49" s="23"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="B50" s="20"/>
+      <c r="C50" s="23"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B51" s="20"/>
+      <c r="C51" s="23"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B52" s="20"/>
+      <c r="C52" s="23"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B53" s="20"/>
+      <c r="C53" s="23"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B54" s="20"/>
+      <c r="C54" s="23"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B55" s="20"/>
+      <c r="C55" s="23"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B56" s="20"/>
+      <c r="C56" s="23"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B57" s="20"/>
+      <c r="C57" s="23"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B58" s="20"/>
+      <c r="C58" s="23"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B59" s="20"/>
+      <c r="C59" s="23"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B60" s="20"/>
+      <c r="C60" s="23"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B61" s="20"/>
+      <c r="C61" s="23"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B62" s="20"/>
+      <c r="C62" s="23"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63" s="20"/>
+      <c r="C63" s="23"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B64" s="20"/>
+      <c r="C64" s="23"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="19" t="s">
+        <v>133</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
upd table for temp and I2C sensor operation
</commit_message>
<xml_diff>
--- a/doc/Serial_Packets.xlsx
+++ b/doc/Serial_Packets.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WORK\Projects\Astrohn\Astrohn_S_DOC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WORK\Projects\Astrohn\git_rep\FTDIDeviceControl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7815"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Packet Format" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="116">
   <si>
     <t>SYNC_1 = 0x5A</t>
   </si>
@@ -348,15 +348,6 @@
     <t>0x001C</t>
   </si>
   <si>
-    <t>0x001D</t>
-  </si>
-  <si>
-    <t>0x001E</t>
-  </si>
-  <si>
-    <t>0x001F</t>
-  </si>
-  <si>
     <t>0x8</t>
   </si>
   <si>
@@ -367,6 +358,21 @@
   </si>
   <si>
     <t>ошибка записи  EPCS</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>temp = (val&gt;&gt;6)/4</t>
+  </si>
+  <si>
+    <t>Sensor I2C</t>
+  </si>
+  <si>
+    <t>Write address</t>
+  </si>
+  <si>
+    <t>Write data (iniatiates I2C operation)</t>
   </si>
 </sst>
 </file>
@@ -672,6 +678,12 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -687,12 +699,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -979,7 +985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -997,16 +1003,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -1145,16 +1151,16 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
@@ -1314,31 +1320,31 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F33" s="13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G33" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F34" s="13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G34" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="26" t="s">
+      <c r="A39" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
     </row>
     <row r="40" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
@@ -1392,16 +1398,16 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="26" t="s">
+      <c r="A48" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B48" s="26"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="26"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="28"/>
+      <c r="H48" s="28"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
@@ -1494,12 +1500,12 @@
       <c r="F52" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I52" s="29" t="s">
+      <c r="I52" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="J52" s="30"/>
-      <c r="K52" s="30"/>
-      <c r="L52" s="31"/>
+      <c r="J52" s="32"/>
+      <c r="K52" s="32"/>
+      <c r="L52" s="33"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F53" s="13" t="s">
@@ -1507,16 +1513,16 @@
       </c>
     </row>
     <row r="56" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="26" t="s">
+      <c r="A56" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="B56" s="26"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
-      <c r="F56" s="26"/>
-      <c r="G56" s="26"/>
-      <c r="H56" s="26"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="28"/>
+      <c r="G56" s="28"/>
+      <c r="H56" s="28"/>
     </row>
     <row r="57" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
@@ -1589,10 +1595,10 @@
         <v>80</v>
       </c>
       <c r="F60" s="13"/>
-      <c r="I60" s="27"/>
-      <c r="J60" s="27"/>
-      <c r="K60" s="27"/>
-      <c r="L60" s="27"/>
+      <c r="I60" s="29"/>
+      <c r="J60" s="29"/>
+      <c r="K60" s="29"/>
+      <c r="L60" s="29"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F61" s="13"/>
@@ -1616,8 +1622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1782,7 +1788,7 @@
       <c r="A19" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="26" t="s">
         <v>90</v>
       </c>
       <c r="C19" s="23" t="s">
@@ -1793,7 +1799,7 @@
       <c r="A20" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="27" t="s">
         <v>93</v>
       </c>
       <c r="C20" s="23" t="s">
@@ -1865,44 +1871,54 @@
       <c r="C28" s="23"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="23"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="25"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="23"/>
+        <v>104</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="23"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="25"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="23"/>
+        <v>105</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="23"/>
+        <v>106</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
-        <v>109</v>
-      </c>
+      <c r="A34" s="19"/>
       <c r="B34" s="20"/>
       <c r="C34" s="23"/>
     </row>

</xml_diff>